<commit_message>
Update Library Database - Data Entry.xlsx
</commit_message>
<xml_diff>
--- a/Library Database - Data Entry.xlsx
+++ b/Library Database - Data Entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilapamukuntla/Documents/Github/LibraryDatabaseSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA4C7F7-8C51-F245-9A2A-B847CB17138B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF19C8CB-3CEA-D546-A975-8C446A0BF151}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" activeTab="2" xr2:uid="{336C36ED-47A3-487C-862D-5D354DE9DA3C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" activeTab="1" xr2:uid="{336C36ED-47A3-487C-862D-5D354DE9DA3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Librarian" sheetId="10" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Author" sheetId="4" r:id="rId5"/>
     <sheet name="Publisher" sheetId="5" r:id="rId6"/>
     <sheet name="Member" sheetId="6" r:id="rId7"/>
-    <sheet name="Email" sheetId="11" r:id="rId8"/>
+    <sheet name="Member_Info" sheetId="11" r:id="rId8"/>
     <sheet name="Book_Return" sheetId="7" r:id="rId9"/>
     <sheet name="Book_Overdue" sheetId="8" r:id="rId10"/>
     <sheet name="Book_Loan" sheetId="9" r:id="rId11"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="251">
   <si>
     <t>Employee_ID</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Assistant</t>
   </si>
   <si>
-    <t>Bernie</t>
-  </si>
-  <si>
     <t>Sanders</t>
   </si>
   <si>
@@ -377,16 +374,424 @@
     <t>Brave New World</t>
   </si>
   <si>
-    <t>Science fiction</t>
-  </si>
-  <si>
     <t>https://www.worldcat.org/title/brave-new-world/oclc/74490211</t>
   </si>
   <si>
     <t>0060850523 9780060850524</t>
   </si>
   <si>
-    <t>Print</t>
+    <t>New York Dover Publications</t>
+  </si>
+  <si>
+    <t>Random House</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>HarperCollins Children's Books</t>
+  </si>
+  <si>
+    <t>Modern Library</t>
+  </si>
+  <si>
+    <t>Harper Perennial Modern Classics</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Heidi</t>
+  </si>
+  <si>
+    <t>9780735822276 0735822271</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/heidi/oclc/774130890?referer=di&amp;ht=edition</t>
+  </si>
+  <si>
+    <t>Science Fiction</t>
+  </si>
+  <si>
+    <t>Les Misérables</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/miserables/oclc/3991366</t>
+  </si>
+  <si>
+    <t>0679600124 9780679600121</t>
+  </si>
+  <si>
+    <t>To Kill a Mockingbird</t>
+  </si>
+  <si>
+    <t>0397001517 9780397001514</t>
+  </si>
+  <si>
+    <t>The Wizard of Oz</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/to-kill-a-mockingbird/oclc/276976</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/wizard-of-oz/oclc/8280289</t>
+  </si>
+  <si>
+    <t>0030616611 9780030616617</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>The Great Gatsby</t>
+  </si>
+  <si>
+    <t>9780743273565 0743273567</t>
+  </si>
+  <si>
+    <t>Romance</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/great-gatsby/oclc/57215622</t>
+  </si>
+  <si>
+    <t>Ulysses</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/ulysses/oclc/25831869</t>
+  </si>
+  <si>
+    <t>0679600116 9780679600114</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>The Grapes of Wrath</t>
+  </si>
+  <si>
+    <t>0143039431 9780143039433</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>A Brief History of Time</t>
+  </si>
+  <si>
+    <t>Non-Fiction</t>
+  </si>
+  <si>
+    <t>0553176986 9780553176988</t>
+  </si>
+  <si>
+    <t>https://www.abebooks.com/products/isbn/9780553176988</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>https://www.worldcat.org/title/grapes-of-wrath/oclc/62593827</t>
+  </si>
+  <si>
+    <t>Anne Frank: The Diary of a Young Girl</t>
+  </si>
+  <si>
+    <t>0553296981 9780553296983</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>https://www.abebooks.com/products/isbn/9780553296983</t>
+  </si>
+  <si>
+    <t>The Year of Magical Thinking</t>
+  </si>
+  <si>
+    <t>Memoir</t>
+  </si>
+  <si>
+    <t>https://www.abebooks.com/products/isbn/9780007216857</t>
+  </si>
+  <si>
+    <t>0007216858 9780007216857</t>
+  </si>
+  <si>
+    <t>Silent Spring</t>
+  </si>
+  <si>
+    <t>https://www.abebooks.com/products/isbn/9780618249060</t>
+  </si>
+  <si>
+    <t>0618249060 9780618249060</t>
+  </si>
+  <si>
+    <t>Wild Swans: Three Daughters of China</t>
+  </si>
+  <si>
+    <t>0743246985 9780743246989</t>
+  </si>
+  <si>
+    <t>https://www.abebooks.com/products/isbn/9780743246989</t>
+  </si>
+  <si>
+    <t>Contact Publishing</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Bantam Books</t>
+  </si>
+  <si>
+    <t>North-South Books</t>
+  </si>
+  <si>
+    <t>Hardcover</t>
+  </si>
+  <si>
+    <t>Softcover</t>
+  </si>
+  <si>
+    <t>A. Lacroix, Verboeckhoven &amp; Cie.</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>J. B. Lippincott &amp; Co</t>
+  </si>
+  <si>
+    <t>George M. Hill Company</t>
+  </si>
+  <si>
+    <t>Charles Scribner's Sons</t>
+  </si>
+  <si>
+    <t>Penguin Books</t>
+  </si>
+  <si>
+    <t>Harper Perennial</t>
+  </si>
+  <si>
+    <t>Houghton Mifflin Company</t>
+  </si>
+  <si>
+    <t>Simon &amp; Schuster</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>Courtney</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>Tami</t>
+  </si>
+  <si>
+    <t>Pamela</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Wendy</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Carman</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Culhane</t>
+  </si>
+  <si>
+    <t>Tori</t>
+  </si>
+  <si>
+    <t>Moreer</t>
+  </si>
+  <si>
+    <t>Ronald</t>
+  </si>
+  <si>
+    <t>Marlin</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>c.dean123@gmail.com</t>
+  </si>
+  <si>
+    <t>cyoung@yahoo.com</t>
+  </si>
+  <si>
+    <t>tamiball@gmail.com</t>
+  </si>
+  <si>
+    <t>rice.pamela@yahoo.com</t>
+  </si>
+  <si>
+    <t>wendyr@gmail.com</t>
+  </si>
+  <si>
+    <t>carmantom@gmail.com</t>
+  </si>
+  <si>
+    <t>jimmyculhane@yahoo.com</t>
+  </si>
+  <si>
+    <t>torimo@hotmail.com</t>
+  </si>
+  <si>
+    <t>johnronald@gmail.com</t>
+  </si>
+  <si>
+    <t>doemarlin@gmail.com</t>
+  </si>
+  <si>
+    <t>Autobiography</t>
+  </si>
+  <si>
+    <t>Southern Gothic</t>
+  </si>
+  <si>
+    <t>Biography</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Hawking</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Cervantes</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Dickens</t>
+  </si>
+  <si>
+    <t>Fyodor</t>
+  </si>
+  <si>
+    <t>Dostoevsky</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Aldous</t>
+  </si>
+  <si>
+    <t>Huxley</t>
+  </si>
+  <si>
+    <t>Johanna</t>
+  </si>
+  <si>
+    <t>Spyri</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harper </t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Baum</t>
+  </si>
+  <si>
+    <t>Fitzgerald</t>
+  </si>
+  <si>
+    <t>Steinbeck</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>Didion</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Carson</t>
+  </si>
+  <si>
+    <t>Jung</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>Joyce</t>
+  </si>
+  <si>
+    <t>Ireland</t>
   </si>
 </sst>
 </file>
@@ -428,12 +833,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -449,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -474,6 +885,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -791,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547928EC-AA24-44F1-9E08-D45C16D6B473}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="200" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -818,8 +1244,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="8">
-        <v>106789</v>
+      <c r="A2" s="8" t="s">
+        <v>217</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>33</v>
@@ -906,13 +1332,13 @@
         <v>166795</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -920,10 +1346,10 @@
         <v>176796</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>47</v>
@@ -934,10 +1360,10 @@
         <v>186797</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>47</v>
@@ -948,10 +1374,10 @@
         <v>196798</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>47</v>
@@ -1425,10 +1851,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2268B606-1708-4579-9CEE-5C0F78022AE0}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -1437,9 +1863,10 @@
     <col min="2" max="2" width="14.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="8"/>
     <col min="4" max="4" width="24.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.83203125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
@@ -1455,324 +1882,608 @@
       <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="H1" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="32">
       <c r="A2" s="4">
-        <v>1234</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="4">
-        <v>5474</v>
+        <v>1232</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3879</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>75</v>
+        <v>157</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4">
-        <v>1235</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1244</v>
+        <v>1233</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1112</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
+        <v>152</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" s="4">
-        <v>3948</v>
+        <v>5474</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>106</v>
+        <v>66</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="4">
-        <v>2039</v>
+        <v>1244</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>105</v>
+        <v>66</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4">
-        <v>9454</v>
+        <v>3948</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>110</v>
+      <c r="H6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" s="4">
-        <v>3456</v>
+        <v>2039</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>108</v>
+        <v>71</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4">
-        <v>5675</v>
+        <v>9454</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>108</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4">
-        <v>9385</v>
+        <v>3456</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" t="s">
-        <v>112</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4">
-        <v>1234</v>
+        <v>5675</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="4">
-        <v>5970</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>9385</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" s="4">
-        <v>3948</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>1234</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="4">
-        <v>9087</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>5970</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C14" s="4">
-        <v>2345</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>3948</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="4">
-        <v>4567</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>9087</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4">
+        <v>1246</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2345</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="4">
+        <v>1247</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4567</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="4">
         <v>1248</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4">
         <v>5678</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4">
+      <c r="D18" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="4">
         <v>1249</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="B19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4">
         <v>7893</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4">
+      <c r="D19" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="4">
         <v>1250</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4">
         <v>3424</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4">
+      <c r="D20" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="4">
         <v>1251</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="4">
         <v>5753</v>
       </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4">
+      <c r="D21" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="4">
         <v>1252</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B22" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="4">
+        <v>8989</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="4">
+        <v>1253</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="4">
+        <v>3874</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="4">
+        <v>1254</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="4">
+        <v>9881</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="32">
+      <c r="A25" s="4">
+        <v>1255</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="4">
+        <v>6878</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="4">
+        <v>1256</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2344</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="4">
+        <v>1257</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="4">
         <v>5683</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{850B11A3-62A6-984F-BC7B-BE8BE16B25A1}"/>
-    <hyperlink ref="I5" r:id="rId2" xr:uid="{FA505670-A0ED-C14C-8BCC-6E4FC307140F}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{202B27CC-2516-DB43-9B96-E7B5A8D2BBF2}"/>
-    <hyperlink ref="I6" r:id="rId4" xr:uid="{74E3E727-210B-4D46-9864-751DE94EB309}"/>
-    <hyperlink ref="I9" r:id="rId5" xr:uid="{1EFFFCB4-6140-624B-B7F7-99CA39C1B7B7}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{850B11A3-62A6-984F-BC7B-BE8BE16B25A1}"/>
+    <hyperlink ref="I7" r:id="rId2" xr:uid="{FA505670-A0ED-C14C-8BCC-6E4FC307140F}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{202B27CC-2516-DB43-9B96-E7B5A8D2BBF2}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{74E3E727-210B-4D46-9864-751DE94EB309}"/>
+    <hyperlink ref="I11" r:id="rId5" xr:uid="{1EFFFCB4-6140-624B-B7F7-99CA39C1B7B7}"/>
+    <hyperlink ref="I13" r:id="rId6" xr:uid="{777D7478-444F-1E46-91F7-C953E309FE23}"/>
+    <hyperlink ref="I14" r:id="rId7" xr:uid="{C098ADFF-45AD-F341-BAD9-E87E1BAE666A}"/>
+    <hyperlink ref="I16" r:id="rId8" xr:uid="{5F330CEA-DB4A-684A-A592-14E2471BD816}"/>
+    <hyperlink ref="I17" r:id="rId9" xr:uid="{21D0ED9D-94F6-2C40-B12A-81DD2201D677}"/>
+    <hyperlink ref="I20" r:id="rId10" xr:uid="{C9214E57-D2D5-2B44-BCC6-D5A4B4597A2B}"/>
+    <hyperlink ref="I27" r:id="rId11" xr:uid="{45F60E1F-A021-5A4D-8EA7-4A602D1C76FB}"/>
+    <hyperlink ref="I3" r:id="rId12" xr:uid="{4403F651-5D32-2141-BC81-DC7765CA72D6}"/>
+    <hyperlink ref="I22" r:id="rId13" xr:uid="{1593C447-75A3-6D45-B2C7-4B8E915178ED}"/>
+    <hyperlink ref="I2" r:id="rId14" xr:uid="{61BC878E-F3E3-4C4A-9BB2-B52D91FDBBAA}"/>
+    <hyperlink ref="I23" r:id="rId15" xr:uid="{27BE8DB1-B5CA-E448-950C-EEAF2A05058D}"/>
+    <hyperlink ref="I24" r:id="rId16" xr:uid="{A7540261-2EB8-5844-B7BF-92E1EB26DA9A}"/>
+    <hyperlink ref="I25" r:id="rId17" xr:uid="{2F948A7F-D1C4-BF45-8BD7-85B3C6A98F3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1780,17 +2491,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3D4419-521A-4711-AB1C-1A1053356953}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1817,15 +2528,395 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="32">
       <c r="A2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2">
+        <v>1947</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2">
+        <v>7564</v>
+      </c>
+      <c r="G2">
+        <v>9908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3">
+        <v>16.97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3">
+        <v>1988</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3">
+        <v>3847</v>
+      </c>
+      <c r="G3">
+        <v>9879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4">
+        <v>9.99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4">
+        <v>1605</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>7854</v>
+      </c>
+      <c r="G4">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
+      <c r="B5">
+        <v>11.99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5">
+        <v>1993</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="11">
+        <v>6711</v>
+      </c>
+      <c r="G5">
+        <v>9898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>11.17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6">
+        <v>2009</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="11">
+        <v>6711</v>
+      </c>
+      <c r="G6">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7">
+        <v>3.85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7">
+        <v>1950</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7">
+        <v>6856</v>
+      </c>
+      <c r="G7">
+        <v>9596</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8">
+        <v>11.55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8">
+        <v>1932</v>
+      </c>
+      <c r="E8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8">
+        <v>7001</v>
+      </c>
+      <c r="G8">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9">
+        <v>2010</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9">
+        <v>7145</v>
+      </c>
+      <c r="G9">
+        <v>9433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10">
+        <v>22.95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10">
+        <v>1862</v>
+      </c>
+      <c r="E10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="11">
+        <v>6711</v>
+      </c>
+      <c r="G10">
+        <v>9123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11">
+        <v>20.99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11">
+        <v>1960</v>
+      </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11">
+        <v>7290</v>
+      </c>
+      <c r="G11">
+        <v>9321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12">
+        <v>20.11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12">
+        <v>1900</v>
+      </c>
+      <c r="E12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12">
+        <v>7435</v>
+      </c>
+      <c r="G12">
+        <v>9456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13">
+        <v>1953</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13">
+        <v>7854</v>
+      </c>
+      <c r="G13">
+        <v>9591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14">
+        <v>12.29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14">
+        <v>2006</v>
+      </c>
+      <c r="E14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="11">
+        <v>7580</v>
+      </c>
+      <c r="G14">
+        <v>9726</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15">
+        <v>2006</v>
+      </c>
+      <c r="E15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15">
+        <v>7725</v>
+      </c>
+      <c r="G15">
+        <v>9861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16">
+        <v>3.98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16">
+        <v>2002</v>
+      </c>
+      <c r="E16" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16">
+        <v>3847</v>
+      </c>
+      <c r="G16">
+        <v>9996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="32">
+      <c r="A17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17">
+        <v>9.32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17">
+        <v>2003</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17">
+        <v>7869</v>
+      </c>
+      <c r="G17">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18">
+        <v>22.28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18">
+        <v>1992</v>
+      </c>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18">
+        <v>8014</v>
+      </c>
+      <c r="G18">
+        <v>1026</v>
       </c>
     </row>
   </sheetData>
@@ -1835,13 +2926,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A333A68B-0059-403C-82CD-FB85142D0B9E}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1855,6 +2950,188 @@
       </c>
       <c r="D1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>7564</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>3847</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>7854</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11">
+        <v>6711</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>6856</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>7001</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7145</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>7290</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>7435</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="11">
+        <v>7580</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>7725</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>7869</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>8014</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1864,13 +3141,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C289AAB-8F71-4DD5-BC1B-09F706C8F8CB}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="184" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1884,6 +3167,230 @@
       </c>
       <c r="D1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1432</v>
+      </c>
+      <c r="B2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1342</v>
+      </c>
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>1252</v>
+      </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>1162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1072</v>
+      </c>
+      <c r="B6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>9821</v>
+      </c>
+      <c r="B7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>8921</v>
+      </c>
+      <c r="B8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>1802</v>
+      </c>
+      <c r="B9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>7121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>6221</v>
+      </c>
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>9467</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>1167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>1388</v>
+      </c>
+      <c r="B14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>1609</v>
+      </c>
+      <c r="B15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>1830</v>
+      </c>
+      <c r="B16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C16" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>2051</v>
+      </c>
+      <c r="B17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1893,16 +3400,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D809AA38-0CC1-4FCA-A686-0D43D44BAAE8}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1914,6 +3422,193 @@
       </c>
       <c r="C1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>9908</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>9879</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3746</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>9898</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>2466</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>9596</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>4536</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>9433</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>9321</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>9456</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>9591</v>
+      </c>
+      <c r="B13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>9726</v>
+      </c>
+      <c r="B14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>9861</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>9996</v>
+      </c>
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1013</v>
+      </c>
+      <c r="B17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>1026</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1923,10 +3618,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FDEEC8-FEC4-4544-BB77-19669D3B9F4B}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="276" zoomScaleNormal="276" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="170" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -1948,7 +3643,7 @@
         <v>967594</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1956,7 +3651,7 @@
         <v>967595</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1964,7 +3659,7 @@
         <v>967596</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1972,7 +3667,7 @@
         <v>967597</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1980,7 +3675,7 @@
         <v>967598</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1988,7 +3683,7 @@
         <v>967599</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1996,7 +3691,7 @@
         <v>967600</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2004,7 +3699,7 @@
         <v>967601</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2012,7 +3707,87 @@
         <v>967602</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>967603</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>967604</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>967605</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>967606</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>967607</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>967608</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>967609</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>967610</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>967611</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>967612</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2026,6 +3801,16 @@
     <hyperlink ref="B8" r:id="rId7" xr:uid="{F74D0E8B-96CD-E647-A51A-AEE8E9766F91}"/>
     <hyperlink ref="B9" r:id="rId8" xr:uid="{043315D8-0301-8042-B3E3-52014BD5A615}"/>
     <hyperlink ref="B10" r:id="rId9" xr:uid="{4AB611A6-F591-5A41-9AFE-62B317B70356}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{3D9CB2BB-37EE-5B49-8273-22B465C1BC7A}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{41F145C9-6223-6F4B-9D30-931B41F88655}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{6130BB83-FE09-0B40-A936-D53291A1FF8D}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{D9DA65BC-18FD-574A-85A5-3EC564978BA9}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{45B4EE4F-24B9-1641-A325-DA9588425A4F}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{BEBE4CF8-7C2E-E844-AED8-7CED3F7A0AA1}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{39E16006-315D-DE41-A20E-B5ADF8C95E43}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{56801AC5-F003-9C4B-9DFC-5DF4E625DA8E}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{AA112956-B39E-B247-AE5F-B07CD783EAFA}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{BDC1450F-B79C-8747-819B-5E22316E0DEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2033,10 +3818,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71931B07-E081-4814-A951-F7485B1E400A}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -2066,155 +3851,325 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
       </c>
       <c r="D2">
         <v>5166555901</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
         <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
       </c>
       <c r="D3">
         <v>5163213456</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>5164376840</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
         <v>86</v>
-      </c>
-      <c r="C5" t="s">
-        <v>87</v>
       </c>
       <c r="D5">
         <v>5160989098</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
         <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
       </c>
       <c r="D6">
         <v>5167483948</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
         <v>93</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
       </c>
       <c r="D7">
         <v>5164382938</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
         <v>96</v>
-      </c>
-      <c r="C8" t="s">
-        <v>97</v>
       </c>
       <c r="D8">
         <v>5168399595</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
         <v>99</v>
-      </c>
-      <c r="C9" t="s">
-        <v>100</v>
       </c>
       <c r="D9">
         <v>5168575744</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
         <v>102</v>
-      </c>
-      <c r="C10" t="s">
-        <v>103</v>
       </c>
       <c r="D10">
         <v>5168493904</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11">
+        <v>5168584056.6666698</v>
+      </c>
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12">
+        <v>5168631211.1666698</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>5168678365.6666698</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14">
+        <v>5168725520.1666698</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15">
+        <v>5168772674.6666698</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16">
+        <v>5168819829.1666698</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17">
+        <v>5168866983.6666698</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18">
+        <v>5168914138.1666698</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>5168961292.6666698</v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20">
+        <v>5169008447.1666698</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2228,6 +4183,16 @@
     <hyperlink ref="A8" r:id="rId7" xr:uid="{1D9F85A9-C114-F141-B3B8-F30234CC5B4B}"/>
     <hyperlink ref="A9" r:id="rId8" xr:uid="{7E115A93-9C26-AC42-B4D5-D39434851F8B}"/>
     <hyperlink ref="A10" r:id="rId9" xr:uid="{BA488B69-1300-FF4F-A190-01E94390E4CA}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{451DF595-8639-5143-97B6-2398E1AE4B96}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{52F0108E-6EB0-6F44-8EB1-CDDD6F115EE6}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{D760FE8D-9AC0-014F-8335-893378EC9D55}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{F2C3C76D-C6C0-D348-9D8E-EED24FFB4893}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{FC1D0A48-1371-5C42-B67E-4ABC4533F081}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{801BEF87-EBCE-D54A-8259-B745C299781A}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{B120DB52-F0E5-1E4B-9502-2A0456D2B24A}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{66152978-8F6A-4A4E-9736-CE01BB4A9C72}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{8054D30F-6922-0D45-B847-34F3E1D7AD65}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{C174CF3A-6407-4F4A-8C38-9D5CE6AAA379}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2238,7 +4203,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>

</xml_diff>